<commit_message>
edited pocet MS na uroven programu
</commit_message>
<xml_diff>
--- a/postprocessing/TEMPLATE_pocet_MS_na_uroven_programu_iba_hlavne_2023_v2024.2.xlsx
+++ b/postprocessing/TEMPLATE_pocet_MS_na_uroven_programu_iba_hlavne_2023_v2024.2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthgovsk.sharepoint.com/sites/OSN445/Shared Documents/General/11_Dátové súbory a prevodníky/02_Užitočné prepočty/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\olve\mzsr\OSN-public\postprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_97E7DD5733A5C581D62915A718E729DA0734C592" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8038A035-2FB0-453B-B7D3-9F4091D791D5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Počet HP na úroveň MS,nemocnice" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -317,8 +316,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,7 +599,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
     <cellStyle name="Percentá" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -938,17 +937,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5703125" style="1" customWidth="1"/>
     <col min="2" max="37" width="7.140625" style="1" customWidth="1"/>
@@ -956,7 +955,7 @@
     <col min="44" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1016,7 @@
       <c r="AP1" s="28"/>
       <c r="AQ1" s="29"/>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>5</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -1366,7 +1365,7 @@
       <c r="AP4" s="26"/>
       <c r="AQ4" s="26"/>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -1485,31 +1484,31 @@
         <v>0</v>
       </c>
       <c r="AL5" s="26">
-        <f t="shared" ref="AL4:AL67" si="8">AF5/SUM($AF5:$AK5)</f>
+        <f t="shared" ref="AL5:AL67" si="8">AF5/SUM($AF5:$AK5)</f>
         <v>0</v>
       </c>
       <c r="AM5" s="26">
-        <f t="shared" ref="AM4:AM67" si="9">AG5/SUM($AF5:$AK5)</f>
+        <f t="shared" ref="AM5:AM67" si="9">AG5/SUM($AF5:$AK5)</f>
         <v>0.94508136094674555</v>
       </c>
       <c r="AN5" s="26">
-        <f t="shared" ref="AN4:AN67" si="10">AH5/SUM($AF5:$AK5)</f>
+        <f t="shared" ref="AN5:AN67" si="10">AH5/SUM($AF5:$AK5)</f>
         <v>4.4907016060862212E-2</v>
       </c>
       <c r="AO5" s="26">
-        <f t="shared" ref="AO4:AO67" si="11">AI5/SUM($AF5:$AK5)</f>
+        <f t="shared" ref="AO5:AO67" si="11">AI5/SUM($AF5:$AK5)</f>
         <v>1.0011622992392223E-2</v>
       </c>
       <c r="AP5" s="26">
-        <f t="shared" ref="AP4:AP67" si="12">AJ5/SUM($AF5:$AK5)</f>
+        <f t="shared" ref="AP5:AP67" si="12">AJ5/SUM($AF5:$AK5)</f>
         <v>0</v>
       </c>
       <c r="AQ5" s="26">
-        <f t="shared" ref="AQ4:AQ67" si="13">AK5/SUM($AF5:$AK5)</f>
+        <f t="shared" ref="AQ5:AQ67" si="13">AK5/SUM($AF5:$AK5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>2</v>
       </c>
@@ -1581,7 +1580,7 @@
       <c r="AP6" s="26"/>
       <c r="AQ6" s="26"/>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
@@ -1724,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>3</v>
       </c>
@@ -1790,7 +1789,7 @@
       <c r="AP8" s="26"/>
       <c r="AQ8" s="26"/>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>11</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>4</v>
       </c>
@@ -2008,7 +2007,7 @@
       <c r="AP10" s="26"/>
       <c r="AQ10" s="26"/>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>12</v>
       </c>
@@ -2151,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>5</v>
       </c>
@@ -2220,7 +2219,7 @@
       <c r="AP12" s="26"/>
       <c r="AQ12" s="26"/>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>6</v>
       </c>
@@ -2438,7 +2437,7 @@
       <c r="AP14" s="26"/>
       <c r="AQ14" s="26"/>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
@@ -2581,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>7</v>
       </c>
@@ -2650,7 +2649,7 @@
       <c r="AP16" s="26"/>
       <c r="AQ16" s="26"/>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>15</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>8</v>
       </c>
@@ -2862,7 +2861,7 @@
       <c r="AP18" s="26"/>
       <c r="AQ18" s="26"/>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>16</v>
       </c>
@@ -3005,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>9</v>
       </c>
@@ -3077,7 +3076,7 @@
       <c r="AP20" s="26"/>
       <c r="AQ20" s="26"/>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>17</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="22">
         <v>10</v>
       </c>
@@ -3298,7 +3297,7 @@
       <c r="AP22" s="26"/>
       <c r="AQ22" s="26"/>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>18</v>
       </c>
@@ -3441,7 +3440,7 @@
         <v>3.263920621450486E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
         <v>11</v>
       </c>
@@ -3519,7 +3518,7 @@
       <c r="AP24" s="26"/>
       <c r="AQ24" s="26"/>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>19</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>12</v>
       </c>
@@ -3725,7 +3724,7 @@
       <c r="AP26" s="26"/>
       <c r="AQ26" s="26"/>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>20</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="22">
         <v>13</v>
       </c>
@@ -3940,7 +3939,7 @@
       <c r="AP28" s="26"/>
       <c r="AQ28" s="26"/>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>21</v>
       </c>
@@ -4083,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <v>14</v>
       </c>
@@ -4140,7 +4139,7 @@
       <c r="AP30" s="26"/>
       <c r="AQ30" s="26"/>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>22</v>
       </c>
@@ -4283,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <v>15</v>
       </c>
@@ -4355,7 +4354,7 @@
       <c r="AP32" s="26"/>
       <c r="AQ32" s="26"/>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>23</v>
       </c>
@@ -4498,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
         <v>16</v>
       </c>
@@ -4579,7 +4578,7 @@
       <c r="AP34" s="26"/>
       <c r="AQ34" s="26"/>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>24</v>
       </c>
@@ -4722,7 +4721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>17</v>
       </c>
@@ -4800,7 +4799,7 @@
       <c r="AP36" s="26"/>
       <c r="AQ36" s="26"/>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>25</v>
       </c>
@@ -4943,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>18</v>
       </c>
@@ -5018,7 +5017,7 @@
       <c r="AP38" s="26"/>
       <c r="AQ38" s="26"/>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>26</v>
       </c>
@@ -5161,7 +5160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:43">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>19</v>
       </c>
@@ -5227,7 +5226,7 @@
       <c r="AP40" s="26"/>
       <c r="AQ40" s="26"/>
     </row>
-    <row r="41" spans="1:43">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>27</v>
       </c>
@@ -5370,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:43">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>20</v>
       </c>
@@ -5439,7 +5438,7 @@
       <c r="AP42" s="26"/>
       <c r="AQ42" s="26"/>
     </row>
-    <row r="43" spans="1:43">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>28</v>
       </c>
@@ -5582,7 +5581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:43">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>21</v>
       </c>
@@ -5648,7 +5647,7 @@
       <c r="AP44" s="26"/>
       <c r="AQ44" s="26"/>
     </row>
-    <row r="45" spans="1:43">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>29</v>
       </c>
@@ -5785,7 +5784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
         <v>22</v>
       </c>
@@ -5851,7 +5850,7 @@
       <c r="AP46" s="26"/>
       <c r="AQ46" s="26"/>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>30</v>
       </c>
@@ -5994,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
         <v>23</v>
       </c>
@@ -6060,7 +6059,7 @@
       <c r="AP48" s="26"/>
       <c r="AQ48" s="26"/>
     </row>
-    <row r="49" spans="1:43">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>31</v>
       </c>
@@ -6203,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:43">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
         <v>24</v>
       </c>
@@ -6275,7 +6274,7 @@
       <c r="AP50" s="26"/>
       <c r="AQ50" s="26"/>
     </row>
-    <row r="51" spans="1:43">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
         <v>32</v>
       </c>
@@ -6418,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
         <v>25</v>
       </c>
@@ -6487,7 +6486,7 @@
       <c r="AP52" s="26"/>
       <c r="AQ52" s="26"/>
     </row>
-    <row r="53" spans="1:43">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>33</v>
       </c>
@@ -6630,7 +6629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
         <v>26</v>
       </c>
@@ -6705,7 +6704,7 @@
       <c r="AP54" s="26"/>
       <c r="AQ54" s="26"/>
     </row>
-    <row r="55" spans="1:43">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>34</v>
       </c>
@@ -6848,7 +6847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" s="22">
         <v>27</v>
       </c>
@@ -6923,7 +6922,7 @@
       <c r="AP56" s="26"/>
       <c r="AQ56" s="26"/>
     </row>
-    <row r="57" spans="1:43">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>35</v>
       </c>
@@ -7066,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A58" s="22">
         <v>28</v>
       </c>
@@ -7141,7 +7140,7 @@
       <c r="AP58" s="26"/>
       <c r="AQ58" s="26"/>
     </row>
-    <row r="59" spans="1:43">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
         <v>36</v>
       </c>
@@ -7284,7 +7283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:43">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A60" s="22">
         <v>29</v>
       </c>
@@ -7353,7 +7352,7 @@
       <c r="AP60" s="26"/>
       <c r="AQ60" s="26"/>
     </row>
-    <row r="61" spans="1:43">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
         <v>37</v>
       </c>
@@ -7496,7 +7495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:43">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" s="22">
         <v>30</v>
       </c>
@@ -7562,7 +7561,7 @@
       <c r="AP62" s="26"/>
       <c r="AQ62" s="26"/>
     </row>
-    <row r="63" spans="1:43">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
         <v>38</v>
       </c>
@@ -7705,7 +7704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:43">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A64" s="22">
         <v>31</v>
       </c>
@@ -7771,7 +7770,7 @@
       <c r="AP64" s="26"/>
       <c r="AQ64" s="26"/>
     </row>
-    <row r="65" spans="1:43">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
         <v>39</v>
       </c>
@@ -7914,7 +7913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:43">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A66" s="22">
         <v>32</v>
       </c>
@@ -7989,7 +7988,7 @@
       <c r="AP66" s="26"/>
       <c r="AQ66" s="26"/>
     </row>
-    <row r="67" spans="1:43">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
         <v>40</v>
       </c>
@@ -8132,7 +8131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:43">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A68" s="22">
         <v>33</v>
       </c>
@@ -8192,7 +8191,7 @@
       <c r="AP68" s="26"/>
       <c r="AQ68" s="26"/>
     </row>
-    <row r="69" spans="1:43">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
         <v>41</v>
       </c>
@@ -8311,31 +8310,31 @@
         <v>0</v>
       </c>
       <c r="AL69" s="26">
-        <f t="shared" ref="AL68:AL131" si="20">AF69/SUM($AF69:$AK69)</f>
+        <f t="shared" ref="AL69:AL131" si="20">AF69/SUM($AF69:$AK69)</f>
         <v>0</v>
       </c>
       <c r="AM69" s="26">
-        <f t="shared" ref="AM68:AM131" si="21">AG69/SUM($AF69:$AK69)</f>
+        <f t="shared" ref="AM69:AM131" si="21">AG69/SUM($AF69:$AK69)</f>
         <v>0</v>
       </c>
       <c r="AN69" s="26">
-        <f t="shared" ref="AN68:AN131" si="22">AH69/SUM($AF69:$AK69)</f>
+        <f t="shared" ref="AN69:AN131" si="22">AH69/SUM($AF69:$AK69)</f>
         <v>1</v>
       </c>
       <c r="AO69" s="26">
-        <f t="shared" ref="AO68:AO131" si="23">AI69/SUM($AF69:$AK69)</f>
+        <f t="shared" ref="AO69:AO131" si="23">AI69/SUM($AF69:$AK69)</f>
         <v>0</v>
       </c>
       <c r="AP69" s="26">
-        <f t="shared" ref="AP68:AP131" si="24">AJ69/SUM($AF69:$AK69)</f>
+        <f t="shared" ref="AP69:AP131" si="24">AJ69/SUM($AF69:$AK69)</f>
         <v>0</v>
       </c>
       <c r="AQ69" s="26">
-        <f t="shared" ref="AQ68:AQ131" si="25">AK69/SUM($AF69:$AK69)</f>
+        <f t="shared" ref="AQ69:AQ131" si="25">AK69/SUM($AF69:$AK69)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:43">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A70" s="22">
         <v>34</v>
       </c>
@@ -8395,7 +8394,7 @@
       <c r="AP70" s="26"/>
       <c r="AQ70" s="26"/>
     </row>
-    <row r="71" spans="1:43">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
         <v>42</v>
       </c>
@@ -8538,7 +8537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:43">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A72" s="22">
         <v>35</v>
       </c>
@@ -8607,7 +8606,7 @@
       <c r="AP72" s="26"/>
       <c r="AQ72" s="26"/>
     </row>
-    <row r="73" spans="1:43">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
         <v>43</v>
       </c>
@@ -8744,7 +8743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:43">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A74" s="22">
         <v>36</v>
       </c>
@@ -8801,7 +8800,7 @@
       <c r="AP74" s="26"/>
       <c r="AQ74" s="26"/>
     </row>
-    <row r="75" spans="1:43">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
         <v>44</v>
       </c>
@@ -8944,7 +8943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:43">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A76" s="22">
         <v>37</v>
       </c>
@@ -9004,7 +9003,7 @@
       <c r="AP76" s="26"/>
       <c r="AQ76" s="26"/>
     </row>
-    <row r="77" spans="1:43">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">
         <v>45</v>
       </c>
@@ -9147,7 +9146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:43">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" s="22">
         <v>38</v>
       </c>
@@ -9222,7 +9221,7 @@
       <c r="AP78" s="26"/>
       <c r="AQ78" s="26"/>
     </row>
-    <row r="79" spans="1:43">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>46</v>
       </c>
@@ -9365,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:43">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A80" s="22">
         <v>39</v>
       </c>
@@ -9412,7 +9411,7 @@
       <c r="AP80" s="26"/>
       <c r="AQ80" s="26"/>
     </row>
-    <row r="81" spans="1:43">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A81" s="22" t="s">
         <v>47</v>
       </c>
@@ -9555,7 +9554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:43">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A82" s="22">
         <v>40</v>
       </c>
@@ -9624,7 +9623,7 @@
       <c r="AP82" s="26"/>
       <c r="AQ82" s="26"/>
     </row>
-    <row r="83" spans="1:43">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A83" s="22" t="s">
         <v>48</v>
       </c>
@@ -9767,7 +9766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:43">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A84" s="22">
         <v>41</v>
       </c>
@@ -9811,7 +9810,7 @@
       <c r="AP84" s="26"/>
       <c r="AQ84" s="26"/>
     </row>
-    <row r="85" spans="1:43">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A85" s="22" t="s">
         <v>49</v>
       </c>
@@ -9954,7 +9953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:43">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A86" s="22">
         <v>42</v>
       </c>
@@ -9986,7 +9985,7 @@
       <c r="AP86" s="26"/>
       <c r="AQ86" s="26"/>
     </row>
-    <row r="87" spans="1:43">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
         <v>50</v>
       </c>
@@ -10129,7 +10128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:43">
+    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A88" s="22">
         <v>43</v>
       </c>
@@ -10192,7 +10191,7 @@
       <c r="AP88" s="26"/>
       <c r="AQ88" s="26"/>
     </row>
-    <row r="89" spans="1:43">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A89" s="22" t="s">
         <v>51</v>
       </c>
@@ -10335,7 +10334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:43">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A90" s="22">
         <v>44</v>
       </c>
@@ -10404,7 +10403,7 @@
       <c r="AP90" s="26"/>
       <c r="AQ90" s="26"/>
     </row>
-    <row r="91" spans="1:43">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A91" s="22" t="s">
         <v>52</v>
       </c>
@@ -10547,7 +10546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:43">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A92" s="22">
         <v>45</v>
       </c>
@@ -10616,7 +10615,7 @@
       <c r="AP92" s="26"/>
       <c r="AQ92" s="26"/>
     </row>
-    <row r="93" spans="1:43">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A93" s="22" t="s">
         <v>53</v>
       </c>
@@ -10753,7 +10752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:43">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A94" s="22">
         <v>46</v>
       </c>
@@ -10786,7 +10785,7 @@
       <c r="AP94" s="26"/>
       <c r="AQ94" s="26"/>
     </row>
-    <row r="95" spans="1:43">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A95" s="22" t="s">
         <v>54</v>
       </c>
@@ -10923,7 +10922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:43">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A96" s="22">
         <v>47</v>
       </c>
@@ -11001,7 +11000,7 @@
       <c r="AP96" s="26"/>
       <c r="AQ96" s="26"/>
     </row>
-    <row r="97" spans="1:43">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A97" s="22" t="s">
         <v>55</v>
       </c>
@@ -11144,7 +11143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:43">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A98" s="22">
         <v>48</v>
       </c>
@@ -11182,7 +11181,7 @@
       <c r="AP98" s="26"/>
       <c r="AQ98" s="26"/>
     </row>
-    <row r="99" spans="1:43">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A99" s="22" t="s">
         <v>56</v>
       </c>
@@ -11325,7 +11324,7 @@
         <v>2.5119316754584274E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:43">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A100" s="22">
         <v>49</v>
       </c>
@@ -11372,7 +11371,7 @@
       <c r="AP100" s="26"/>
       <c r="AQ100" s="26"/>
     </row>
-    <row r="101" spans="1:43">
+    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A101" s="22" t="s">
         <v>57</v>
       </c>
@@ -11515,7 +11514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:43">
+    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A102" s="22">
         <v>50</v>
       </c>
@@ -11590,7 +11589,7 @@
       <c r="AP102" s="26"/>
       <c r="AQ102" s="26"/>
     </row>
-    <row r="103" spans="1:43">
+    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A103" s="22" t="s">
         <v>58</v>
       </c>
@@ -11733,7 +11732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:43">
+    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A104" s="22">
         <v>51</v>
       </c>
@@ -11808,7 +11807,7 @@
       <c r="AP104" s="26"/>
       <c r="AQ104" s="26"/>
     </row>
-    <row r="105" spans="1:43">
+    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A105" s="22" t="s">
         <v>59</v>
       </c>
@@ -11951,7 +11950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:43">
+    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A106" s="22">
         <v>52</v>
       </c>
@@ -12026,7 +12025,7 @@
       <c r="AP106" s="26"/>
       <c r="AQ106" s="26"/>
     </row>
-    <row r="107" spans="1:43">
+    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>60</v>
       </c>
@@ -12169,7 +12168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:43">
+    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A108" s="22">
         <v>53</v>
       </c>
@@ -12244,7 +12243,7 @@
       <c r="AP108" s="26"/>
       <c r="AQ108" s="26"/>
     </row>
-    <row r="109" spans="1:43">
+    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
         <v>61</v>
       </c>
@@ -12387,7 +12386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:43">
+    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A110" s="22">
         <v>54</v>
       </c>
@@ -12462,7 +12461,7 @@
       <c r="AP110" s="26"/>
       <c r="AQ110" s="26"/>
     </row>
-    <row r="111" spans="1:43">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A111" s="22" t="s">
         <v>62</v>
       </c>
@@ -12605,7 +12604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:43">
+    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A112" s="22">
         <v>55</v>
       </c>
@@ -12668,7 +12667,7 @@
       <c r="AP112" s="26"/>
       <c r="AQ112" s="26"/>
     </row>
-    <row r="113" spans="1:43">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A113" s="22" t="s">
         <v>63</v>
       </c>
@@ -12811,7 +12810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:43">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A114" s="22">
         <v>56</v>
       </c>
@@ -12886,7 +12885,7 @@
       <c r="AP114" s="26"/>
       <c r="AQ114" s="26"/>
     </row>
-    <row r="115" spans="1:43">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A115" s="22" t="s">
         <v>64</v>
       </c>
@@ -13029,7 +13028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:43">
+    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A116" s="22">
         <v>57</v>
       </c>
@@ -13101,7 +13100,7 @@
       <c r="AP116" s="26"/>
       <c r="AQ116" s="26"/>
     </row>
-    <row r="117" spans="1:43">
+    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A117" s="22" t="s">
         <v>65</v>
       </c>
@@ -13244,7 +13243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:43">
+    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A118" s="22">
         <v>58</v>
       </c>
@@ -13322,7 +13321,7 @@
       <c r="AP118" s="26"/>
       <c r="AQ118" s="26"/>
     </row>
-    <row r="119" spans="1:43">
+    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A119" s="22" t="s">
         <v>66</v>
       </c>
@@ -13465,7 +13464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:43">
+    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A120" s="22">
         <v>59</v>
       </c>
@@ -13537,7 +13536,7 @@
       <c r="AP120" s="26"/>
       <c r="AQ120" s="26"/>
     </row>
-    <row r="121" spans="1:43">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A121" s="22" t="s">
         <v>67</v>
       </c>
@@ -13680,7 +13679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:43">
+    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A122" s="22">
         <v>60</v>
       </c>
@@ -13749,7 +13748,7 @@
       <c r="AP122" s="26"/>
       <c r="AQ122" s="26"/>
     </row>
-    <row r="123" spans="1:43">
+    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A123" s="22" t="s">
         <v>68</v>
       </c>
@@ -13892,7 +13891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:43">
+    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A124" s="22">
         <v>61</v>
       </c>
@@ -13964,7 +13963,7 @@
       <c r="AP124" s="26"/>
       <c r="AQ124" s="26"/>
     </row>
-    <row r="125" spans="1:43">
+    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A125" s="22" t="s">
         <v>69</v>
       </c>
@@ -14107,7 +14106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:43">
+    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A126" s="22">
         <v>62</v>
       </c>
@@ -14182,7 +14181,7 @@
       <c r="AP126" s="26"/>
       <c r="AQ126" s="26"/>
     </row>
-    <row r="127" spans="1:43">
+    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>70</v>
       </c>
@@ -14325,7 +14324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:43">
+    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A128" s="22">
         <v>63</v>
       </c>
@@ -14394,7 +14393,7 @@
       <c r="AP128" s="26"/>
       <c r="AQ128" s="26"/>
     </row>
-    <row r="129" spans="1:43">
+    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A129" s="22" t="s">
         <v>71</v>
       </c>
@@ -14537,7 +14536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:43">
+    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A130" s="22">
         <v>64</v>
       </c>
@@ -14606,7 +14605,7 @@
       <c r="AP130" s="26"/>
       <c r="AQ130" s="26"/>
     </row>
-    <row r="131" spans="1:43">
+    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A131" s="22" t="s">
         <v>72</v>
       </c>
@@ -14749,7 +14748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:43">
+    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
         <v>65</v>
       </c>
@@ -14827,7 +14826,7 @@
       <c r="AP132" s="26"/>
       <c r="AQ132" s="26"/>
     </row>
-    <row r="133" spans="1:43">
+    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A133" s="22" t="s">
         <v>73</v>
       </c>
@@ -14946,31 +14945,31 @@
         <v>0</v>
       </c>
       <c r="AL133" s="26">
-        <f t="shared" ref="AL132:AL160" si="32">AF133/SUM($AF133:$AK133)</f>
+        <f t="shared" ref="AL133:AL159" si="32">AF133/SUM($AF133:$AK133)</f>
         <v>0</v>
       </c>
       <c r="AM133" s="26">
-        <f t="shared" ref="AM132:AM160" si="33">AG133/SUM($AF133:$AK133)</f>
+        <f t="shared" ref="AM133:AM159" si="33">AG133/SUM($AF133:$AK133)</f>
         <v>0.59510410804727065</v>
       </c>
       <c r="AN133" s="26">
-        <f t="shared" ref="AN132:AN160" si="34">AH133/SUM($AF133:$AK133)</f>
+        <f t="shared" ref="AN133:AN159" si="34">AH133/SUM($AF133:$AK133)</f>
         <v>0.32517351341211781</v>
       </c>
       <c r="AO133" s="26">
-        <f t="shared" ref="AO132:AO160" si="35">AI133/SUM($AF133:$AK133)</f>
+        <f t="shared" ref="AO133:AO159" si="35">AI133/SUM($AF133:$AK133)</f>
         <v>7.9722378540611524E-2</v>
       </c>
       <c r="AP133" s="26">
-        <f t="shared" ref="AP132:AP160" si="36">AJ133/SUM($AF133:$AK133)</f>
+        <f t="shared" ref="AP133:AP159" si="36">AJ133/SUM($AF133:$AK133)</f>
         <v>0</v>
       </c>
       <c r="AQ133" s="26">
-        <f t="shared" ref="AQ132:AQ160" si="37">AK133/SUM($AF133:$AK133)</f>
+        <f t="shared" ref="AQ133:AQ159" si="37">AK133/SUM($AF133:$AK133)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:43">
+    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
         <v>66</v>
       </c>
@@ -15039,7 +15038,7 @@
       <c r="AP134" s="26"/>
       <c r="AQ134" s="26"/>
     </row>
-    <row r="135" spans="1:43">
+    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A135" s="22" t="s">
         <v>74</v>
       </c>
@@ -15182,7 +15181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:43">
+    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
         <v>67</v>
       </c>
@@ -15254,7 +15253,7 @@
       <c r="AP136" s="26"/>
       <c r="AQ136" s="26"/>
     </row>
-    <row r="137" spans="1:43">
+    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A137" s="22" t="s">
         <v>75</v>
       </c>
@@ -15397,7 +15396,7 @@
         <v>2.4905660377358491E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:43">
+    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A138" s="22">
         <v>68</v>
       </c>
@@ -15463,7 +15462,7 @@
       <c r="AP138" s="26"/>
       <c r="AQ138" s="26"/>
     </row>
-    <row r="139" spans="1:43">
+    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A139" s="22" t="s">
         <v>76</v>
       </c>
@@ -15606,7 +15605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:43">
+    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A140" s="22">
         <v>69</v>
       </c>
@@ -15672,7 +15671,7 @@
       <c r="AP140" s="26"/>
       <c r="AQ140" s="26"/>
     </row>
-    <row r="141" spans="1:43">
+    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A141" s="22" t="s">
         <v>77</v>
       </c>
@@ -15815,7 +15814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:43">
+    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A142" s="22">
         <v>70</v>
       </c>
@@ -15881,7 +15880,7 @@
       <c r="AP142" s="26"/>
       <c r="AQ142" s="26"/>
     </row>
-    <row r="143" spans="1:43">
+    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A143" s="22" t="s">
         <v>78</v>
       </c>
@@ -16024,7 +16023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:43">
+    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A144" s="22">
         <v>71</v>
       </c>
@@ -16099,7 +16098,7 @@
       <c r="AP144" s="26"/>
       <c r="AQ144" s="26"/>
     </row>
-    <row r="145" spans="1:43">
+    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A145" s="22" t="s">
         <v>79</v>
       </c>
@@ -16242,7 +16241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:43">
+    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A146" s="22">
         <v>72</v>
       </c>
@@ -16308,7 +16307,7 @@
       <c r="AP146" s="26"/>
       <c r="AQ146" s="26"/>
     </row>
-    <row r="147" spans="1:43">
+    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A147" s="22" t="s">
         <v>80</v>
       </c>
@@ -16451,7 +16450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:43">
+    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A148" s="22">
         <v>73</v>
       </c>
@@ -16526,7 +16525,7 @@
       <c r="AP148" s="26"/>
       <c r="AQ148" s="26"/>
     </row>
-    <row r="149" spans="1:43">
+    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A149" s="22" t="s">
         <v>81</v>
       </c>
@@ -16669,7 +16668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:43">
+    <row r="150" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A150" s="22">
         <v>74</v>
       </c>
@@ -16747,7 +16746,7 @@
       <c r="AP150" s="26"/>
       <c r="AQ150" s="26"/>
     </row>
-    <row r="151" spans="1:43">
+    <row r="151" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A151" s="22" t="s">
         <v>82</v>
       </c>
@@ -16890,7 +16889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:43">
+    <row r="152" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A152" s="22">
         <v>75</v>
       </c>
@@ -16922,7 +16921,7 @@
       <c r="AP152" s="26"/>
       <c r="AQ152" s="26"/>
     </row>
-    <row r="153" spans="1:43">
+    <row r="153" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A153" s="22" t="s">
         <v>83</v>
       </c>
@@ -17065,7 +17064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:43">
+    <row r="154" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A154" s="22">
         <v>76</v>
       </c>
@@ -17137,7 +17136,7 @@
       <c r="AP154" s="26"/>
       <c r="AQ154" s="26"/>
     </row>
-    <row r="155" spans="1:43">
+    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A155" s="22" t="s">
         <v>84</v>
       </c>
@@ -17274,7 +17273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:43">
+    <row r="156" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A156" s="22">
         <v>77</v>
       </c>
@@ -17337,7 +17336,7 @@
       <c r="AP156" s="26"/>
       <c r="AQ156" s="26"/>
     </row>
-    <row r="157" spans="1:43">
+    <row r="157" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A157" s="22" t="s">
         <v>85</v>
       </c>
@@ -17480,7 +17479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:43">
+    <row r="158" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A158" s="22">
         <v>98</v>
       </c>
@@ -17513,7 +17512,7 @@
       <c r="AP158" s="26"/>
       <c r="AQ158" s="26"/>
     </row>
-    <row r="159" spans="1:43">
+    <row r="159" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A159" s="22" t="s">
         <v>86</v>
       </c>
@@ -17656,7 +17655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:43">
+    <row r="160" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A160" s="23">
         <v>99</v>
       </c>
@@ -17713,7 +17712,7 @@
       <c r="AP160" s="26"/>
       <c r="AQ160" s="26"/>
     </row>
-    <row r="161" spans="1:43">
+    <row r="161" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
         <v>1</v>
       </c>
@@ -17868,7 +17867,7 @@
       <c r="AP161" s="26"/>
       <c r="AQ161" s="26"/>
     </row>
-    <row r="162" spans="1:43">
+    <row r="162" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
         <v>2</v>
       </c>
@@ -18023,7 +18022,7 @@
       <c r="AP162" s="26"/>
       <c r="AQ162" s="26"/>
     </row>
-    <row r="163" spans="1:43">
+    <row r="163" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A163" s="24" t="s">
         <v>87</v>
       </c>
@@ -18064,11 +18063,12 @@
       <c r="AP163" s="26"/>
       <c r="AQ163" s="26"/>
     </row>
-    <row r="164" spans="1:43">
+    <row r="164" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>88</v>
       </c>
       <c r="B164" s="2">
+        <f>SUM(B61)</f>
         <v>484</v>
       </c>
       <c r="C164" s="1">
@@ -18087,9 +18087,11 @@
         <v>0</v>
       </c>
       <c r="H164" s="2">
+        <f>SUM(H147:H148,H103:H104,H61:H62,H57:H58,H21:H24,H17:H18)</f>
         <v>40798</v>
       </c>
       <c r="I164" s="1">
+        <f>SUM(I145:I148,I141:I142,I127:I138,I103:I104,I97:I98,I75:I76,I71:I72,I65:I66,I49:I60,I33:I36,I27:I28,I21:I24,I17:I18,I5:I6)</f>
         <v>174780</v>
       </c>
       <c r="J164" s="1">
@@ -18105,12 +18107,15 @@
         <v>0</v>
       </c>
       <c r="N164" s="2">
+        <f>SUM(N147:N148,N125:N126,N103:N104,N61:N62,N57:N58,N39:N40,N29:N32,N17:N24,N11:N12)</f>
         <v>41803</v>
       </c>
       <c r="O164" s="1">
+        <f>SUM(O141:O148,O127:O138,O103:O104,O97:O98,O75:O78,O71:O72,O49:O68,O27:O36,O17:O24,O5:O6)</f>
         <v>107322</v>
       </c>
       <c r="P164" s="1">
+        <f>SUM(P153:P154,P145:P148,P139:P140,P125:P136,P103:P104,P99:P100,P87:P88,P75:P76,P71:P72,P47:P66,P43:P44,P39:P40,P27:P30,P17:P24,P9:P14,P5:P6)</f>
         <v>18216</v>
       </c>
       <c r="Q164" s="1">
@@ -18123,15 +18128,19 @@
         <v>0</v>
       </c>
       <c r="T164" s="2">
+        <f>SUM(T147:T148,T125:T126,T103:T104,T57:T58,T61:T62,T39:T40,T29:T32,T17:T24,T11:T12,)</f>
         <v>14902</v>
       </c>
       <c r="U164" s="1">
+        <f>SUM(U141:U148,U127:U138,U103:U104,U97:U98,U81:U82,U75:U78,U71:U72,U49:U68,U27:U36,U17:U24,U5:U6,)</f>
         <v>57050</v>
       </c>
       <c r="V164" s="1">
-        <v>27499</v>
+        <f>SUM(V125:V148,V99:V100,V87:V88,V81:V84,V75:V76,V47:V72,V39:V44,V17:V34,V5:V14)</f>
+        <v>27385</v>
       </c>
       <c r="W164" s="1">
+        <f>SUM(W153:W154,W147:W148,W137:W142,W131:W134,W125:W128,W103:W104,W99:W100,W81:W82,W77:W78,W71:W72,W65:W66,W51:W62,W47:W48,W35:W44,W27:W28,W17:W24,W5:W12)</f>
         <v>4011</v>
       </c>
       <c r="X164" s="1">
@@ -18141,18 +18150,23 @@
         <v>0</v>
       </c>
       <c r="Z164" s="2">
+        <f>SUM(Z147:Z148,Z125:Z126,Z103:Z104,Z61:Z62,Z57:Z58,Z39:Z40,Z29:Z32,Z17:Z24,Z11:Z12)</f>
         <v>14658</v>
       </c>
       <c r="AA164" s="1">
+        <f>SUM(AA141:AA148,AA127:AA138,AA103:AA104,AA97:AA98,AA81:AA82,AA75:AA78,AA71:AA72,AA49:AA68,AA27:AA36,AA17:AA24,AA5:AA6)</f>
         <v>56378</v>
       </c>
       <c r="AB164" s="1">
+        <f>SUM(AB125:AB150,AB103:AB104,AB99:AB100,AB87:AB88,AB81:AB84,AB75:AB76,AB47:AB72,AB39:AB44,AB5:AB34)</f>
         <v>22141</v>
       </c>
       <c r="AC164" s="1">
+        <f>SUM(AC151:AC154,AC145:AC148,AC125:AC142,AC103:AC104,AC99:AC100,AC81:AC86,AC77:AC78,AC71:AC72,AC65:AC66,AC51:AC62,AC47:AC48,AC35:AC44,AC31:AC32,AC27:AC28,AC5:AC24,)</f>
         <v>8007</v>
       </c>
       <c r="AD164" s="1">
+        <f>SUM(AD147:AD148,AD141:AD142,AD135:AD136,AD129:AD132,AD125:AD126,AD103:AD104,AD81:AD82,AD65:AD66,AD57:AD58,AD53:AD54,AD31:AD38,AD27:AD28,AD19:AD24,AD15:AD16,AD9:AD10,)</f>
         <v>740</v>
       </c>
       <c r="AE164" s="3">
@@ -18165,17 +18179,19 @@
       <c r="AP164" s="26"/>
       <c r="AQ164" s="26"/>
     </row>
-    <row r="165" spans="1:43">
+    <row r="165" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B165" s="2">
+        <f>SUM(B23,B147)</f>
         <v>175</v>
       </c>
       <c r="C165" s="1">
         <v>0</v>
       </c>
       <c r="D165" s="1">
+        <f>SUM(D153:D154,D87:D88)</f>
         <v>26</v>
       </c>
       <c r="E165" s="1">
@@ -18191,15 +18207,19 @@
         <v>0</v>
       </c>
       <c r="I165" s="1">
+        <f>SUM(I143:I144,I87:I88,I81:I82,I77:I78,I67:I68,I61:I64,I29:I32,I19:I20,)</f>
         <v>24165</v>
       </c>
       <c r="J165" s="1">
+        <f>SUM(J153:J154,J141:J148,J125:J138,J103:J104,J99:J100,J87:J88,J81:J84,J75:J76,J49:J72,J41:J42,J17:J32,J9:J12,J5:J6,)</f>
         <v>14427</v>
       </c>
       <c r="K165" s="1">
+        <f>SUM(K99:K100,K21:K24,)</f>
         <v>176</v>
       </c>
       <c r="L165" s="1">
+        <f>SUM(L33:L34)</f>
         <v>61</v>
       </c>
       <c r="M165" s="3">
@@ -18209,15 +18229,19 @@
         <v>0</v>
       </c>
       <c r="O165" s="1">
+        <f>SUM(O81:O82)</f>
         <v>7621</v>
       </c>
       <c r="P165" s="1">
+        <f>SUM(P149:P150,P141:P144,P137:P138,P79:P84,P67:P70,P41:P42,P31:P34,P25:P26,P15:P16,P7:P8,)</f>
         <v>9327</v>
       </c>
       <c r="Q165" s="1">
+        <f>SUM(Q151:Q154,Q145:Q148,Q125:Q140,Q103:Q104,Q99:Q100,Q81:Q86,Q77:Q78,Q65:Q66,Q71:Q72,Q51:Q62,Q35:Q44,Q31:Q32,Q27:Q28,Q17:Q24,Q5:Q14,)</f>
         <v>3484</v>
       </c>
       <c r="R165" s="1">
+        <f>SUM(R131:R132,)</f>
         <v>2</v>
       </c>
       <c r="S165" s="3">
@@ -18230,12 +18254,15 @@
         <v>0</v>
       </c>
       <c r="V165" s="1">
+        <f>SUM(V149:V150,V79:V80,V15:V16)</f>
         <v>560</v>
       </c>
       <c r="W165" s="1">
+        <f>SUM(W151:W152,W145:W146,W135:W136,W129:W130,W83:W86,W31:W32,W13:W16)</f>
         <v>408</v>
       </c>
       <c r="X165" s="1">
+        <f>SUM(X147:X148,X135:X136,X131:X132,X125:X126,X103:X104,X63:X66,X53:X58,X31:X36,X19:X24,X15:X16,X9:X10,)</f>
         <v>16</v>
       </c>
       <c r="Y165" s="3">
@@ -18248,12 +18275,14 @@
         <v>0</v>
       </c>
       <c r="AB165" s="1">
+        <f>SUM(AB79:AB80,)</f>
         <v>454</v>
       </c>
       <c r="AC165" s="1">
         <v>0</v>
       </c>
       <c r="AD165" s="1">
+        <f>SUM(AD143:AD144,AD67:AD68,AD63:AD64,AD55:AD56,)</f>
         <v>9</v>
       </c>
       <c r="AE165" s="3">
@@ -18266,20 +18295,24 @@
       <c r="AP165" s="26"/>
       <c r="AQ165" s="26"/>
     </row>
-    <row r="166" spans="1:43">
+    <row r="166" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A166" s="15" t="s">
         <v>90</v>
       </c>
       <c r="B166" s="2">
+        <f>SUM(B153:B159,B149,B101:B145,B87:B96,B81:B82,B63:B78,B25:B60,B3:B22)</f>
         <v>56113</v>
       </c>
       <c r="C166" s="1">
+        <f>SUM(C153:C156,C147:C150,C139:C140,C131:C134,C121:C128,C117:C118,C101:C114,C95:C98,C87:C92,C69:C80,C63:C66,C51:C60,C33:C48,C27:C28,C21:C24,C3:C18)</f>
         <v>104443</v>
       </c>
       <c r="D166" s="1">
+        <f>SUM(D149:D150,D123:D124,D117:D118,D95:D96,D77:D78,D35:D38,)</f>
         <v>526</v>
       </c>
       <c r="E166" s="1">
+        <f>SUM(E155:E156,E149:E150,E143:E144,E95:E96,E77:E78,E49:E50,E33:E34)</f>
         <v>7</v>
       </c>
       <c r="F166" s="1">
@@ -18289,15 +18322,19 @@
         <v>0</v>
       </c>
       <c r="H166" s="2">
+        <f>SUM(H153:H160,H149:H150,H105:H146,H101:H102,H87:H96,H81:H82,H63:H78,H59:H60,H25:H56,H19:H20,H3:H16)</f>
         <v>60720</v>
       </c>
       <c r="I166" s="1">
+        <f>SUM(I153:I156,I149:I150,I139:I140,I105:I126,I101:I102,I95:I96,I89:I92,I79:I80,I73:I74,I69:I70,I37:I48,I7:I16,I3:I4)</f>
         <v>16598</v>
       </c>
       <c r="J166" s="1">
+        <f>SUM(J149:J150,J113:J124,J105:J108,J101:J102,J95:J96,J89:J92,J77:J78,J47:J48,J35:J38,J3:J4)</f>
         <v>2986</v>
       </c>
       <c r="K166" s="1">
+        <f>SUM(K155:K156,K149:K150,K143:K144,K95:K96,K49:K50,K33:K34,)</f>
         <v>0</v>
       </c>
       <c r="L166" s="1">
@@ -18307,152 +18344,197 @@
         <v>0</v>
       </c>
       <c r="N166" s="2">
+        <f>SUM(N153:N160,N149:N150,N127:N146,N105:N124,N101:N102,N87:N96,N81:N82,N63:N78,N59:N60,N41:N56,N33:N38,N25:N28,N13:N16,N3:N10)</f>
         <v>59555</v>
       </c>
       <c r="O166" s="1">
+        <f>SUM(O153:O156,O149:O150,O139:O140,O105:O126,O101:O102,O95:O96,O87:O92,O79:O80,O73:O74,O69:O70,O37:O48,O25:O26,O7:O16,O3:O4)</f>
         <v>6063</v>
       </c>
       <c r="P166" s="1">
+        <f>SUM(P105:P124,P101:P102,P95:P96,P89:P92,P77:P78,P45:P46,P35:P38,P3:P4)</f>
         <v>3218</v>
       </c>
       <c r="Q166" s="1">
+        <f>SUM(Q155:Q156,Q149:Q150,Q143:Q144,Q113:Q124,Q105:Q110,Q101:Q102,Q95:Q96,Q89:Q92,Q73:Q74,Q49:Q50,Q45:Q46,Q33:Q34,Q25:Q26,Q3:Q4)</f>
         <v>2100</v>
       </c>
       <c r="R166" s="1">
+        <f>SUM(R109:R110,R13:R14)</f>
         <v>0</v>
       </c>
       <c r="S166" s="3">
         <v>0</v>
       </c>
       <c r="T166" s="2">
+        <f>SUM(T153:T160,T149:T150,T127:T146,T105:T124,T101:T102,T87:T96,T81:T82,T63:T78,T59:T60,T41:T56,T33:T38,T25:T28,T13:T16,T3:T10,)</f>
         <v>19205</v>
       </c>
       <c r="U166" s="1">
+        <f>SUM(U153:U156,U149:U150,U139:U140,U105:U126,U101:U102,U95:U96,U87:U92,U79:U80,U73:U74,U69:U70,U37:U48,U25:U26,U7:U16,U3:U4)</f>
         <v>3784</v>
       </c>
       <c r="V166" s="1">
+        <f>SUM(V153:V154,V105:V124,V101:V102,V95:V96,V89:V92,V77:V78,V45:V46,V35:V38,V3:V4)</f>
         <v>2214</v>
       </c>
       <c r="W166" s="1">
+        <f>SUM(W155:W156,W149:W150,W143:W144,W105:W124,W101:W102,W95:W96,W89:W92,W73:W74,W49:W50,W45:W46,W33:W34,W25:W26,W3:W4)</f>
         <v>2390</v>
       </c>
       <c r="X166" s="1">
+        <f>SUM(X113:X120,X105:X110,X101:X102,X13:X14,X3:X4)</f>
         <v>10</v>
       </c>
       <c r="Y166" s="3">
         <v>0</v>
       </c>
       <c r="Z166" s="2">
+        <f>SUM(Z153:Z160,Z149:Z150,Z127:Z146,Z105:Z124,Z101:Z102,Z87:Z96,Z81:Z82,Z63:Z78,Z59:Z60,Z41:Z56,Z33:Z38,Z25:Z28,Z13:Z16,Z3:Z10)</f>
         <v>23530</v>
       </c>
       <c r="AA166" s="1">
+        <f>SUM(AA153:AA156,AA149:AA150,AA139:AA140,AA105:AA126,AA101:AA102,AA95:AA96,AA87:AA92,AA79:AA80,AA73:AA74,AA69:AA70,AA37:AA48,AA25:AA26,AA7:AA16,AA3:AA4)</f>
         <v>6559</v>
       </c>
       <c r="AB166" s="1">
+        <f>SUM(AB153:AB154,AB105:AB124,AB101:AB102,AB95:AB96,AB89:AB92,AB77:AB78,AB45:AB46,AB35:AB38,AB3:AB4)</f>
         <v>3220</v>
       </c>
       <c r="AC166" s="1">
+        <f>SUM(AC155:AC156,AC149:AC150,AC143:AC144, AC105:AC124,AC101:AC102,AC95:AC96,AC89:AC92,AC73:AC74,AC49:AC50,AC45:AC46,AC33:AC34,AC25:AC26,AC3:AC4)</f>
         <v>2026</v>
       </c>
       <c r="AD166" s="1">
+        <f>SUM(AD113:AD120,AD101:AD110,AD13:AD14,AD3:AD6)</f>
         <v>84</v>
       </c>
       <c r="AE166" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:43">
+    <row r="167" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A167" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B167" s="4">
+      <c r="B167" s="5">
+        <f>B161-SUM(B164:B166)</f>
         <v>0</v>
       </c>
       <c r="C167" s="5">
+        <f>C161-SUM(C164:C166)</f>
         <v>9631</v>
       </c>
       <c r="D167" s="5">
+        <f t="shared" ref="D167:AE167" si="51">D161-SUM(D164:D166)</f>
         <v>6314</v>
       </c>
       <c r="E167" s="5">
+        <f t="shared" si="51"/>
         <v>1117</v>
       </c>
       <c r="F167" s="5">
+        <f t="shared" si="51"/>
         <v>20</v>
       </c>
       <c r="G167" s="6">
+        <f t="shared" si="51"/>
         <v>3</v>
       </c>
-      <c r="H167" s="4">
+      <c r="H167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="I167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="J167" s="5">
+        <f t="shared" si="51"/>
         <v>3076</v>
       </c>
       <c r="K167" s="5">
+        <f t="shared" si="51"/>
         <v>3779</v>
       </c>
       <c r="L167" s="5">
+        <f t="shared" si="51"/>
         <v>47</v>
       </c>
       <c r="M167" s="6">
+        <f t="shared" si="51"/>
         <v>10</v>
       </c>
-      <c r="N167" s="4">
+      <c r="N167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="P167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="Q167" s="5">
+        <f t="shared" si="51"/>
         <v>312</v>
       </c>
       <c r="R167" s="5">
+        <f t="shared" si="51"/>
         <v>92</v>
       </c>
       <c r="S167" s="6">
+        <f t="shared" si="51"/>
         <v>16</v>
       </c>
-      <c r="T167" s="4">
+      <c r="T167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="U167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="V167" s="5">
-        <v>0</v>
+        <f t="shared" si="51"/>
+        <v>114</v>
       </c>
       <c r="W167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X167" s="5">
+        <f t="shared" si="51"/>
         <v>10</v>
       </c>
       <c r="Y167" s="6">
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
-      <c r="Z167" s="4">
+      <c r="Z167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AA167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AB167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AC167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AD167" s="5">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AE167" s="6">
+        <f t="shared" si="51"/>
         <v>36</v>
       </c>
     </row>
@@ -18467,6 +18549,80 @@
     <mergeCell ref="Z1:AE1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:AE3">
+    <cfRule type="colorScale" priority="170">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:AE5">
+    <cfRule type="colorScale" priority="171">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:AE7">
+    <cfRule type="colorScale" priority="169">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:AE9">
+    <cfRule type="colorScale" priority="168">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:AE11">
+    <cfRule type="colorScale" priority="167">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:AE160">
+    <cfRule type="expression" dxfId="3" priority="174">
+      <formula>ISBLANK(B3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="175">
+      <formula>B3="D"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="176">
+      <formula>B3="P"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="177">
+      <formula>B3 ="N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:AE13">
+    <cfRule type="colorScale" priority="166">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:AE15">
     <cfRule type="colorScale" priority="165">
       <colorScale>
         <cfvo type="min"/>
@@ -18476,17 +18632,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:AE5">
-    <cfRule type="colorScale" priority="166">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:AE7">
+  <conditionalFormatting sqref="B17:AE17">
     <cfRule type="colorScale" priority="164">
       <colorScale>
         <cfvo type="min"/>
@@ -18496,7 +18642,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:AE9">
+  <conditionalFormatting sqref="B19:AE19">
     <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
@@ -18506,7 +18652,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:AE11">
+  <conditionalFormatting sqref="B21:AE21">
     <cfRule type="colorScale" priority="162">
       <colorScale>
         <cfvo type="min"/>
@@ -18516,21 +18662,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:AE160">
-    <cfRule type="expression" dxfId="3" priority="169">
-      <formula>ISBLANK(B3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="170">
-      <formula>B3="D"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="171">
-      <formula>B3="P"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="172">
-      <formula>B3 ="N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:AE13">
+  <conditionalFormatting sqref="B23:AE23">
     <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="min"/>
@@ -18540,7 +18672,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:AE15">
+  <conditionalFormatting sqref="B25:AE25">
     <cfRule type="colorScale" priority="160">
       <colorScale>
         <cfvo type="min"/>
@@ -18550,7 +18682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:AE17">
+  <conditionalFormatting sqref="B27:AE27">
     <cfRule type="colorScale" priority="159">
       <colorScale>
         <cfvo type="min"/>
@@ -18560,7 +18692,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:AE19">
+  <conditionalFormatting sqref="B29:AE29">
     <cfRule type="colorScale" priority="158">
       <colorScale>
         <cfvo type="min"/>
@@ -18570,7 +18702,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:AE21">
+  <conditionalFormatting sqref="B31:AE31">
     <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="min"/>
@@ -18580,7 +18712,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:AE23">
+  <conditionalFormatting sqref="B33:AE33">
     <cfRule type="colorScale" priority="156">
       <colorScale>
         <cfvo type="min"/>
@@ -18590,7 +18722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:AE25">
+  <conditionalFormatting sqref="B35:AE35">
     <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
@@ -18600,7 +18732,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:AE27">
+  <conditionalFormatting sqref="B37:AE37">
     <cfRule type="colorScale" priority="154">
       <colorScale>
         <cfvo type="min"/>
@@ -18610,7 +18742,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:AE29">
+  <conditionalFormatting sqref="B39:AE39">
     <cfRule type="colorScale" priority="153">
       <colorScale>
         <cfvo type="min"/>
@@ -18620,7 +18752,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:AE31">
+  <conditionalFormatting sqref="B41:AE41">
     <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
@@ -18630,7 +18762,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:AE33">
+  <conditionalFormatting sqref="B43:AE43">
     <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="min"/>
@@ -18640,17 +18772,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:AE35">
-    <cfRule type="colorScale" priority="150">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37:AE37">
+  <conditionalFormatting sqref="B47:AE47">
     <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="min"/>
@@ -18660,7 +18782,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:AE39">
+  <conditionalFormatting sqref="B49:AE49">
     <cfRule type="colorScale" priority="148">
       <colorScale>
         <cfvo type="min"/>
@@ -18670,7 +18792,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:AE41">
+  <conditionalFormatting sqref="B51:AE51">
     <cfRule type="colorScale" priority="147">
       <colorScale>
         <cfvo type="min"/>
@@ -18680,7 +18802,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:AE43">
+  <conditionalFormatting sqref="B53:AE53">
     <cfRule type="colorScale" priority="146">
       <colorScale>
         <cfvo type="min"/>
@@ -18690,7 +18812,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47:AE47">
+  <conditionalFormatting sqref="B55:AE55">
+    <cfRule type="colorScale" priority="145">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:AE57">
     <cfRule type="colorScale" priority="144">
       <colorScale>
         <cfvo type="min"/>
@@ -18700,7 +18832,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49:AE49">
+  <conditionalFormatting sqref="B59:AE59">
     <cfRule type="colorScale" priority="143">
       <colorScale>
         <cfvo type="min"/>
@@ -18710,7 +18842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51:AE51">
+  <conditionalFormatting sqref="B61:AE61">
     <cfRule type="colorScale" priority="142">
       <colorScale>
         <cfvo type="min"/>
@@ -18720,7 +18852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53:AE53">
+  <conditionalFormatting sqref="B63:AE63">
     <cfRule type="colorScale" priority="141">
       <colorScale>
         <cfvo type="min"/>
@@ -18730,7 +18862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B55:AE55">
+  <conditionalFormatting sqref="B65:AE65">
     <cfRule type="colorScale" priority="140">
       <colorScale>
         <cfvo type="min"/>
@@ -18740,7 +18872,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57:AE57">
+  <conditionalFormatting sqref="B67:AE67">
     <cfRule type="colorScale" priority="139">
       <colorScale>
         <cfvo type="min"/>
@@ -18750,7 +18882,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59:AE59">
+  <conditionalFormatting sqref="B69:AE69">
     <cfRule type="colorScale" priority="138">
       <colorScale>
         <cfvo type="min"/>
@@ -18760,7 +18892,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61:AE61">
+  <conditionalFormatting sqref="B71:AE71">
     <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
@@ -18770,17 +18902,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B63:AE63">
-    <cfRule type="colorScale" priority="136">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65:AE65">
+  <conditionalFormatting sqref="B75:AE75">
     <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="min"/>
@@ -18790,7 +18912,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:AE67">
+  <conditionalFormatting sqref="B77:AE77">
     <cfRule type="colorScale" priority="134">
       <colorScale>
         <cfvo type="min"/>
@@ -18800,7 +18922,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:AE69">
+  <conditionalFormatting sqref="B79:AE79">
     <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
@@ -18810,7 +18932,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B71:AE71">
+  <conditionalFormatting sqref="B81:AE81">
     <cfRule type="colorScale" priority="132">
       <colorScale>
         <cfvo type="min"/>
@@ -18820,7 +18942,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B75:AE75">
+  <conditionalFormatting sqref="B83:AE83">
+    <cfRule type="colorScale" priority="131">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B85:AE85">
     <cfRule type="colorScale" priority="130">
       <colorScale>
         <cfvo type="min"/>
@@ -18830,7 +18962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77:AE77">
+  <conditionalFormatting sqref="B87:AE87">
     <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
@@ -18840,7 +18972,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79:AE79">
+  <conditionalFormatting sqref="B89:AE89">
     <cfRule type="colorScale" priority="128">
       <colorScale>
         <cfvo type="min"/>
@@ -18850,7 +18982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B81:AE81">
+  <conditionalFormatting sqref="B91:AE91">
     <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
@@ -18860,27 +18992,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B83:AE83">
-    <cfRule type="colorScale" priority="126">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B85:AE85">
-    <cfRule type="colorScale" priority="125">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B87:AE87">
+  <conditionalFormatting sqref="B97:AE97">
     <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min"/>
@@ -18890,7 +19002,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B89:AE89">
+  <conditionalFormatting sqref="B99:AE99">
     <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
@@ -18900,7 +19012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:AE91">
+  <conditionalFormatting sqref="B101:AE101">
     <cfRule type="colorScale" priority="122">
       <colorScale>
         <cfvo type="min"/>
@@ -18910,7 +19022,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B97:AE97">
+  <conditionalFormatting sqref="B103:AE103">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B105:AE105">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B107:AE107">
     <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
@@ -18920,7 +19052,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B99:AE99">
+  <conditionalFormatting sqref="B109:AE109">
     <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="min"/>
@@ -18930,7 +19062,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B101:AE101">
+  <conditionalFormatting sqref="B111:AE111">
     <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="min"/>
@@ -18940,7 +19072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B103:AE103">
+  <conditionalFormatting sqref="B113:AE113">
     <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>
@@ -18950,7 +19082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B105:AE105">
+  <conditionalFormatting sqref="B115:AE115">
     <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
@@ -18960,7 +19092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B107:AE107">
+  <conditionalFormatting sqref="B117:AE117">
     <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="min"/>
@@ -18970,7 +19102,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B109:AE109">
+  <conditionalFormatting sqref="B119:AE119">
     <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="min"/>
@@ -18980,7 +19112,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B111:AE111">
+  <conditionalFormatting sqref="B121:AE121">
     <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
@@ -18990,7 +19122,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B113:AE113">
+  <conditionalFormatting sqref="B123:AE123">
     <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
@@ -19000,7 +19132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B115:AE115">
+  <conditionalFormatting sqref="B125:AE125">
     <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
@@ -19010,7 +19142,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B117:AE117">
+  <conditionalFormatting sqref="B127:AE127">
     <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
@@ -19020,7 +19152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B119:AE119">
+  <conditionalFormatting sqref="B129:AE129">
     <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
@@ -19030,7 +19162,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B121:AE121">
+  <conditionalFormatting sqref="B131:AE131">
     <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
@@ -19040,7 +19172,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B123:AE123">
+  <conditionalFormatting sqref="B133:AE133">
     <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min"/>
@@ -19050,7 +19182,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B125:AE125">
+  <conditionalFormatting sqref="B135:AE135">
     <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
@@ -19060,7 +19192,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B127:AE127">
+  <conditionalFormatting sqref="B137:AE137">
     <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
@@ -19070,7 +19202,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B129:AE129">
+  <conditionalFormatting sqref="B139:AE139">
     <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
@@ -19080,7 +19212,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B131:AE131">
+  <conditionalFormatting sqref="B141:AE141">
     <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min"/>
@@ -19090,7 +19222,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B133:AE133">
+  <conditionalFormatting sqref="B143:AE143">
     <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
@@ -19100,7 +19232,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B135:AE135">
+  <conditionalFormatting sqref="B145:AE145">
     <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="min"/>
@@ -19110,7 +19242,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B137:AE137">
+  <conditionalFormatting sqref="B147:AE147">
     <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
@@ -19120,7 +19252,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B139:AE139">
+  <conditionalFormatting sqref="B149:AE149">
     <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="min"/>
@@ -19130,7 +19262,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B141:AE141">
+  <conditionalFormatting sqref="B151:AE151">
     <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
@@ -19140,7 +19272,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B143:AE143">
+  <conditionalFormatting sqref="B153:AE153">
     <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min"/>
@@ -19150,17 +19282,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B145:AE145">
-    <cfRule type="colorScale" priority="95">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B147:AE147">
+  <conditionalFormatting sqref="B157:AE157">
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
@@ -19170,7 +19292,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B149:AE149">
+  <conditionalFormatting sqref="B159:AE159">
     <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
@@ -19180,8 +19302,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B151:AE151">
-    <cfRule type="colorScale" priority="92">
+  <conditionalFormatting sqref="AF3:AK3">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -19190,17 +19312,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B153:AE153">
-    <cfRule type="colorScale" priority="91">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B157:AE157">
+  <conditionalFormatting sqref="AF5:AK5">
     <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
@@ -19210,7 +19322,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B159:AE159">
+  <conditionalFormatting sqref="B161:G161">
     <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
@@ -19220,7 +19332,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF3:AK3">
+  <conditionalFormatting sqref="H161:M161">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N161:S161">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T161:Y161">
     <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
@@ -19230,7 +19362,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF5:AK5">
+  <conditionalFormatting sqref="Z161:AE161">
     <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
@@ -19240,7 +19372,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B161:G161">
+  <conditionalFormatting sqref="AF161:AK161">
     <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
@@ -19250,7 +19382,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H161:M161">
+  <conditionalFormatting sqref="AF7:AK7">
     <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
@@ -19260,7 +19392,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N161:S161">
+  <conditionalFormatting sqref="AF9:AK9">
     <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
@@ -19270,7 +19402,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T161:Y161">
+  <conditionalFormatting sqref="AF11:AK11">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
@@ -19280,7 +19412,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z161:AE161">
+  <conditionalFormatting sqref="AF13:AK13">
     <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
@@ -19290,7 +19422,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF161:AK161">
+  <conditionalFormatting sqref="AF15:AK15">
     <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
@@ -19300,7 +19432,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF7:AK7">
+  <conditionalFormatting sqref="AF17:AK17">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
@@ -19310,7 +19442,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF9:AK9">
+  <conditionalFormatting sqref="AF19:AK19">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
@@ -19320,7 +19452,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF11:AK11">
+  <conditionalFormatting sqref="AF21:AK21">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -19330,7 +19462,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF13:AK13">
+  <conditionalFormatting sqref="AF23:AK23">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
@@ -19340,7 +19472,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF15:AK15">
+  <conditionalFormatting sqref="AF25:AK25">
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
@@ -19350,7 +19482,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF17:AK17">
+  <conditionalFormatting sqref="AF27:AK27">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
@@ -19360,7 +19492,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF19:AK19">
+  <conditionalFormatting sqref="AF29:AK29">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
@@ -19370,7 +19502,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF21:AK21">
+  <conditionalFormatting sqref="AF31:AK31">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -19380,7 +19512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF23:AK23">
+  <conditionalFormatting sqref="AF33:AK33">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -19390,7 +19522,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF25:AK25">
+  <conditionalFormatting sqref="AF35:AK35">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -19400,7 +19532,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF27:AK27">
+  <conditionalFormatting sqref="AF37:AK37">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -19410,7 +19542,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF29:AK29">
+  <conditionalFormatting sqref="AF39:AK39">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -19420,7 +19552,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF31:AK31">
+  <conditionalFormatting sqref="AF41:AK41">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -19430,7 +19562,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF33:AK33">
+  <conditionalFormatting sqref="AF43:AK43">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -19440,7 +19572,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF35:AK35">
+  <conditionalFormatting sqref="AF47:AK47">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -19450,7 +19582,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF37:AK37">
+  <conditionalFormatting sqref="AF49:AK49">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -19460,7 +19592,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF39:AK39">
+  <conditionalFormatting sqref="AF51:AK51">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -19470,7 +19602,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF41:AK41">
+  <conditionalFormatting sqref="AF53:AK53">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -19480,7 +19612,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF43:AK43">
+  <conditionalFormatting sqref="AF55:AK55">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -19490,7 +19622,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF47:AK47">
+  <conditionalFormatting sqref="AF57:AK57">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -19500,7 +19632,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF49:AK49">
+  <conditionalFormatting sqref="AF59:AK59">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -19510,7 +19642,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF51:AK51">
+  <conditionalFormatting sqref="AF61:AK61">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -19520,7 +19652,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF53:AK53">
+  <conditionalFormatting sqref="AF63:AK63">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -19530,7 +19662,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF55:AK55">
+  <conditionalFormatting sqref="AF65:AK65">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -19540,7 +19672,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF57:AK57">
+  <conditionalFormatting sqref="AF67:AK67">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -19550,7 +19682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF59:AK59">
+  <conditionalFormatting sqref="AF69:AK69">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -19560,7 +19692,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF61:AK61">
+  <conditionalFormatting sqref="AF71:AK71">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -19570,7 +19702,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF63:AK63">
+  <conditionalFormatting sqref="AF75:AK75">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -19580,7 +19712,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF65:AK65">
+  <conditionalFormatting sqref="AF77:AK77">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -19590,7 +19722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF67:AK67">
+  <conditionalFormatting sqref="AF79:AK79">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -19600,7 +19732,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF69:AK69">
+  <conditionalFormatting sqref="AF81:AK81">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -19610,7 +19742,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF71:AK71">
+  <conditionalFormatting sqref="AF83:AK83">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -19620,7 +19752,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF75:AK75">
+  <conditionalFormatting sqref="AF85:AK85">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -19630,7 +19762,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF77:AK77">
+  <conditionalFormatting sqref="AF87:AK87">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -19640,7 +19772,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF79:AK79">
+  <conditionalFormatting sqref="AF89:AK89">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -19650,7 +19782,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF81:AK81">
+  <conditionalFormatting sqref="AF91:AK91">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -19660,7 +19792,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF83:AK83">
+  <conditionalFormatting sqref="AF97:AK97">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -19670,7 +19802,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF85:AK85">
+  <conditionalFormatting sqref="AF99:AK99">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -19680,7 +19812,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF87:AK87">
+  <conditionalFormatting sqref="AF101:AK101">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -19690,7 +19822,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF89:AK89">
+  <conditionalFormatting sqref="AF103:AK103">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -19700,7 +19832,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF91:AK91">
+  <conditionalFormatting sqref="AF105:AK105">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -19710,7 +19842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF97:AK97">
+  <conditionalFormatting sqref="AF107:AK107">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -19720,7 +19852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF99:AK99">
+  <conditionalFormatting sqref="AF109:AK109">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -19730,7 +19862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF101:AK101">
+  <conditionalFormatting sqref="AF111:AK111">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -19740,7 +19872,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF103:AK103">
+  <conditionalFormatting sqref="AF113:AK113">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -19750,7 +19882,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF105:AK105">
+  <conditionalFormatting sqref="AF115:AK115">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -19760,7 +19892,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF107:AK107">
+  <conditionalFormatting sqref="AF117:AK117">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -19770,7 +19902,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF109:AK109">
+  <conditionalFormatting sqref="AF119:AK119">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -19780,7 +19912,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF111:AK111">
+  <conditionalFormatting sqref="AF121:AK121">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -19790,7 +19922,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF113:AK113">
+  <conditionalFormatting sqref="AF123:AK123">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -19800,7 +19932,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF115:AK115">
+  <conditionalFormatting sqref="AF125:AK125">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -19810,7 +19942,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF117:AK117">
+  <conditionalFormatting sqref="AF127:AK127">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -19820,7 +19952,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF119:AK119">
+  <conditionalFormatting sqref="AF129:AK129">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -19830,7 +19962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF121:AK121">
+  <conditionalFormatting sqref="AF131:AK131">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -19840,7 +19972,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF123:AK123">
+  <conditionalFormatting sqref="AF133:AK133">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -19850,7 +19982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF125:AK125">
+  <conditionalFormatting sqref="AF135:AK135">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -19860,7 +19992,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF127:AK127">
+  <conditionalFormatting sqref="AF137:AK137">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -19870,7 +20002,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF129:AK129">
+  <conditionalFormatting sqref="AF139:AK139">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -19880,7 +20012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF131:AK131">
+  <conditionalFormatting sqref="AF141:AK141">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -19890,7 +20022,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF133:AK133">
+  <conditionalFormatting sqref="AF143:AK143">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -19900,7 +20032,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF135:AK135">
+  <conditionalFormatting sqref="AF145:AK145">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -19910,7 +20042,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF137:AK137">
+  <conditionalFormatting sqref="AF147:AK147">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -19920,7 +20052,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF139:AK139">
+  <conditionalFormatting sqref="AF149:AK149">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -19930,7 +20062,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF141:AK141">
+  <conditionalFormatting sqref="AF151:AK151">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -19940,7 +20072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF143:AK143">
+  <conditionalFormatting sqref="AF153:AK153">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -19950,7 +20082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF145:AK145">
+  <conditionalFormatting sqref="AF157:AK157">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -19960,7 +20092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF147:AK147">
+  <conditionalFormatting sqref="AF159:AK159">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -19970,57 +20102,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF149:AK149">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF151:AK151">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF153:AK153">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF157:AK157">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF159:AK159">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B164:G167">
+  <conditionalFormatting sqref="B164:G167 H167:AE167">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -20030,7 +20112,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H164:M167">
+  <conditionalFormatting sqref="H164:M166">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -20040,7 +20122,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N164:S167">
+  <conditionalFormatting sqref="N164:S166">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -20050,7 +20132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T164:Y167">
+  <conditionalFormatting sqref="T164:Y166">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -20060,7 +20142,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z164:AE167">
+  <conditionalFormatting sqref="Z164:AE166">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -20076,18 +20158,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <date xmlns="856c868e-d386-4b40-a6b9-c2d94f442fd3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="3a0606dd-bf36-4def-9284-cd3cc8bb8967" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="856c868e-d386-4b40-a6b9-c2d94f442fd3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006E54E1FCEBA93549AF9D0C94F315E52B" ma:contentTypeVersion="16" ma:contentTypeDescription="Umožňuje vytvoriť nový dokument." ma:contentTypeScope="" ma:versionID="7a60c8105668d593b1f38f3e7b3dae53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="856c868e-d386-4b40-a6b9-c2d94f442fd3" xmlns:ns3="3a0606dd-bf36-4def-9284-cd3cc8bb8967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5ee7ab0433baf672e6b596044b7c3c9" ns2:_="" ns3:_="">
     <xsd:import namespace="856c868e-d386-4b40-a6b9-c2d94f442fd3"/>
@@ -20328,6 +20398,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <date xmlns="856c868e-d386-4b40-a6b9-c2d94f442fd3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="3a0606dd-bf36-4def-9284-cd3cc8bb8967" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="856c868e-d386-4b40-a6b9-c2d94f442fd3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -20338,13 +20420,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2DE8BBF-318D-4EEA-8D48-4754A1A58906}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C4DA36-5C45-4E5F-9460-320573BE77EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="856c868e-d386-4b40-a6b9-c2d94f442fd3"/>
+    <ds:schemaRef ds:uri="3a0606dd-bf36-4def-9284-cd3cc8bb8967"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C4DA36-5C45-4E5F-9460-320573BE77EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2DE8BBF-318D-4EEA-8D48-4754A1A58906}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="856c868e-d386-4b40-a6b9-c2d94f442fd3"/>
+    <ds:schemaRef ds:uri="3a0606dd-bf36-4def-9284-cd3cc8bb8967"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CDD9A13-66EF-4D94-B11B-B1DD1888D645}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CDD9A13-66EF-4D94-B11B-B1DD1888D645}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>